<commit_message>
Se obtienen graficas, y se actualiza ppt
</commit_message>
<xml_diff>
--- a/Rubrica_S1_DM g9.xlsx
+++ b/Rubrica_S1_DM g9.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27618"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uandresbelloedu-my.sharepoint.com/personal/i_gamboaalvarado_uandresbello_edu/Documents/Documents/003_tercerAño_2024/05_mineriaDeDatos/Grupo_9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{1FD4942F-02FD-46DB-92E6-707C9ECE955D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F69A26F6-2CC2-495E-BEB8-441FA5BFCE42}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{1FD4942F-02FD-46DB-92E6-707C9ECE955D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB015537-53DF-46E5-B552-8994A3FC0101}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{48001077-B0FA-43D7-8863-EF925434C9DF}"/>
   </bookViews>
@@ -112,6 +112,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF111111"/>
+        <rFont val="Calibri"/>
+      </rPr>
       <t xml:space="preserve">Presenta el resumen de medidas estadísticas de todas las variables numéricas en una tabla e interpreta cada medida, que incluye: 
 -Cantidad de observaciones y proporción de datos faltantes.
 -Medidas de posición (media, mediana, </t>
@@ -119,9 +124,8 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="7"/>
+        <color rgb="FFFFC000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t>Q1, Q3</t>
     </r>
@@ -153,7 +157,7 @@
   </si>
   <si>
     <t>Aspectos que debe cumplir:
--Describe una variable de tipo entera o categórica, 
+-Describe una variable de tipo entera o categórica, ppt4
 -Identifica claramente cuáles son las categorías de la variable.
 -Representa un gráfico de barra con ponderación de cada categoría 
 -Explica los resultados.</t>
@@ -564,9 +568,8 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="7"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -795,9 +798,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -843,6 +843,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1161,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A5DD04-EA05-47E6-B111-91DD7D53ABF0}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1196,19 +1199,19 @@
       <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="39"/>
+      <c r="H1" s="38"/>
       <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="81.599999999999994" customHeight="1">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -1262,14 +1265,14 @@
       <c r="I3" s="5"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="105">
+    <row r="4" spans="1:10" ht="91.5">
       <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -1295,10 +1298,10 @@
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1324,7 +1327,7 @@
       <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -1349,8 +1352,8 @@
       <c r="I6" s="5"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="105">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:10" ht="120" customHeight="1">
+      <c r="A7" s="39" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="15" t="s">
@@ -1378,14 +1381,14 @@
       <c r="I7" s="7"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="75">
+    <row r="8" spans="1:10" ht="108.75" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>44</v>
       </c>
       <c r="D8" s="17" t="s">
@@ -1407,11 +1410,11 @@
       <c r="I8" s="5"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="90">
+    <row r="9" spans="1:10" ht="105.75" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>49</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -1436,11 +1439,11 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="90">
+    <row r="10" spans="1:10" ht="126" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="34" t="s">
         <v>55</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1465,14 +1468,14 @@
       <c r="I10" s="5"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="135.6" customHeight="1">
+    <row r="11" spans="1:10" ht="168.75" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>59</v>
       </c>
       <c r="D11" s="17" t="s">
@@ -1495,10 +1498,10 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="95.45" customHeight="1">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>61</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1524,13 +1527,13 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="86.45" customHeight="1">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="28" t="s">
         <v>68</v>
       </c>
       <c r="D13" s="17" t="s">
@@ -1553,10 +1556,10 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="75">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="32" t="s">
         <v>73</v>
       </c>
       <c r="C14" s="17" t="s">
@@ -1582,10 +1585,10 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" ht="75">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="25" t="s">
         <v>79</v>
       </c>
       <c r="C15" s="17" t="s">
@@ -1611,10 +1614,10 @@
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:10" ht="30">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="30" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="15" t="s">
@@ -1640,10 +1643,10 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="120">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="30" t="s">
         <v>91</v>
       </c>
       <c r="C17" s="15" t="s">
@@ -1773,7 +1776,7 @@
       </c>
     </row>
     <row r="17" spans="2:2">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="36" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Avances segun la clase 8, y modificaciones post presentacion, falta realizar regresion lineal y avanzar en el arbol de procesos. entro de las tareas pendientes es poder ordenar tanto datos como archivos.
</commit_message>
<xml_diff>
--- a/Rubrica_S1_DM g9.xlsx
+++ b/Rubrica_S1_DM g9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uandresbelloedu-my.sharepoint.com/personal/i_gamboaalvarado_uandresbello_edu/Documents/Documents/003_tercerAño_2024/05_mineriaDeDatos/Grupo_9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{1FD4942F-02FD-46DB-92E6-707C9ECE955D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB015537-53DF-46E5-B552-8994A3FC0101}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{1FD4942F-02FD-46DB-92E6-707C9ECE955D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BE5440E-92C0-4688-8700-DF192B762019}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{48001077-B0FA-43D7-8863-EF925434C9DF}"/>
   </bookViews>
@@ -93,7 +93,7 @@
 -Introducción donde argumente la importancia de minería de datos, según algoritmos supervisados y no supervisados.
 -Descripción de la base de datos ¿qué variables y cuántas? ¿cuántas observaciones?,¿de qué trata la base de datos?
 -Objetivo general
--Objetivos específicos</t>
+-Objetivos específicos  6</t>
   </si>
   <si>
     <t xml:space="preserve">Obtener una mejor prediccion del valor de los diamantes.-                                                     - Que combinaciones de aspectos nos puede brindar el mejor precio // Crear correlación entre variables que puedan predecir el precio // deteccion  en los datos  atipicos o anomalais (estos son propios del dismante) </t>
@@ -572,7 +572,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -648,6 +648,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -730,7 +736,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -838,13 +844,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1164,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A5DD04-EA05-47E6-B111-91DD7D53ABF0}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1199,10 +1208,10 @@
       <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="38"/>
+      <c r="H1" s="39"/>
       <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1240,7 +1249,7 @@
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="40" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="14" t="s">
@@ -1353,7 +1362,7 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="120" customHeight="1">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="15" t="s">

</xml_diff>